<commit_message>
DONE YOU TUBE SCRAP
</commit_message>
<xml_diff>
--- a/youtube_webscrab/Tina Huang.xlsx
+++ b/youtube_webscrab/Tina Huang.xlsx
@@ -489,13 +489,13 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>86325</v>
+        <v>88761</v>
       </c>
       <c r="E2" t="n">
-        <v>4835</v>
+        <v>4930</v>
       </c>
       <c r="F2" t="n">
-        <v>958</v>
+        <v>988</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>45017</v>
@@ -521,10 +521,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>12879</v>
+        <v>12944</v>
       </c>
       <c r="E3" t="n">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="F3" t="n">
         <v>78</v>
@@ -553,10 +553,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>15510</v>
+        <v>15672</v>
       </c>
       <c r="E4" t="n">
-        <v>1252</v>
+        <v>1261</v>
       </c>
       <c r="F4" t="n">
         <v>28</v>
@@ -585,13 +585,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>922907</v>
+        <v>931418</v>
       </c>
       <c r="E5" t="n">
-        <v>38708</v>
+        <v>38916</v>
       </c>
       <c r="F5" t="n">
-        <v>1164</v>
+        <v>1168</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>44987</v>
@@ -617,10 +617,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>38457</v>
+        <v>38507</v>
       </c>
       <c r="E6" t="n">
-        <v>2444</v>
+        <v>2447</v>
       </c>
       <c r="F6" t="n">
         <v>89</v>
@@ -649,10 +649,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>452080</v>
+        <v>452721</v>
       </c>
       <c r="E7" t="n">
-        <v>23548</v>
+        <v>23575</v>
       </c>
       <c r="F7" t="n">
         <v>886</v>
@@ -681,10 +681,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>87458</v>
+        <v>87817</v>
       </c>
       <c r="E8" t="n">
-        <v>5334</v>
+        <v>5350</v>
       </c>
       <c r="F8" t="n">
         <v>245</v>
@@ -713,10 +713,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>636793</v>
+        <v>637319</v>
       </c>
       <c r="E9" t="n">
-        <v>34230</v>
+        <v>34250</v>
       </c>
       <c r="F9" t="n">
         <v>532</v>
@@ -745,10 +745,10 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>411740</v>
+        <v>412186</v>
       </c>
       <c r="E10" t="n">
-        <v>22192</v>
+        <v>22207</v>
       </c>
       <c r="F10" t="n">
         <v>367</v>
@@ -777,10 +777,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>22719</v>
+        <v>22726</v>
       </c>
       <c r="E11" t="n">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="F11" t="n">
         <v>97</v>
@@ -809,10 +809,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>102786</v>
+        <v>102794</v>
       </c>
       <c r="E12" t="n">
-        <v>4833</v>
+        <v>4834</v>
       </c>
       <c r="F12" t="n">
         <v>336</v>
@@ -841,10 +841,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>316383</v>
+        <v>316487</v>
       </c>
       <c r="E13" t="n">
-        <v>20874</v>
+        <v>20877</v>
       </c>
       <c r="F13" t="n">
         <v>626</v>
@@ -873,10 +873,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>86124</v>
+        <v>86175</v>
       </c>
       <c r="E14" t="n">
-        <v>5330</v>
+        <v>5333</v>
       </c>
       <c r="F14" t="n">
         <v>224</v>
@@ -905,13 +905,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>60826</v>
+        <v>60846</v>
       </c>
       <c r="E15" t="n">
-        <v>3311</v>
+        <v>3312</v>
       </c>
       <c r="F15" t="n">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>44831</v>
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>45549</v>
+        <v>45561</v>
       </c>
       <c r="E16" t="n">
         <v>2405</v>
@@ -969,10 +969,10 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>106229</v>
+        <v>106321</v>
       </c>
       <c r="E17" t="n">
-        <v>5948</v>
+        <v>5950</v>
       </c>
       <c r="F17" t="n">
         <v>235</v>
@@ -1001,10 +1001,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>56412</v>
+        <v>56427</v>
       </c>
       <c r="E18" t="n">
-        <v>3096</v>
+        <v>3097</v>
       </c>
       <c r="F18" t="n">
         <v>245</v>
@@ -1033,7 +1033,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>66047</v>
+        <v>66056</v>
       </c>
       <c r="E19" t="n">
         <v>3254</v>
@@ -1065,10 +1065,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>129970</v>
+        <v>130080</v>
       </c>
       <c r="E20" t="n">
-        <v>7260</v>
+        <v>7267</v>
       </c>
       <c r="F20" t="n">
         <v>470</v>
@@ -1097,10 +1097,10 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>69319</v>
+        <v>69346</v>
       </c>
       <c r="E21" t="n">
-        <v>3868</v>
+        <v>3869</v>
       </c>
       <c r="F21" t="n">
         <v>185</v>
@@ -1129,10 +1129,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>229211</v>
+        <v>229228</v>
       </c>
       <c r="E22" t="n">
-        <v>12470</v>
+        <v>12471</v>
       </c>
       <c r="F22" t="n">
         <v>779</v>
@@ -1161,13 +1161,13 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>240387</v>
+        <v>240399</v>
       </c>
       <c r="E23" t="n">
         <v>9933</v>
       </c>
       <c r="F23" t="n">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>44714</v>
@@ -1193,10 +1193,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>115288</v>
+        <v>115322</v>
       </c>
       <c r="E24" t="n">
-        <v>6320</v>
+        <v>6322</v>
       </c>
       <c r="F24" t="n">
         <v>227</v>
@@ -1225,7 +1225,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>95127</v>
+        <v>95172</v>
       </c>
       <c r="E25" t="n">
         <v>4907</v>
@@ -1257,10 +1257,10 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>196379</v>
+        <v>196409</v>
       </c>
       <c r="E26" t="n">
-        <v>11265</v>
+        <v>11266</v>
       </c>
       <c r="F26" t="n">
         <v>288</v>
@@ -1289,7 +1289,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>61371</v>
+        <v>61379</v>
       </c>
       <c r="E27" t="n">
         <v>3657</v>
@@ -1321,10 +1321,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>123850</v>
+        <v>123867</v>
       </c>
       <c r="E28" t="n">
-        <v>5999</v>
+        <v>6000</v>
       </c>
       <c r="F28" t="n">
         <v>284</v>
@@ -1353,7 +1353,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>67495</v>
+        <v>67517</v>
       </c>
       <c r="E29" t="n">
         <v>4088</v>
@@ -1385,10 +1385,10 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>421971</v>
+        <v>422138</v>
       </c>
       <c r="E30" t="n">
-        <v>17166</v>
+        <v>17172</v>
       </c>
       <c r="F30" t="n">
         <v>246</v>
@@ -1417,13 +1417,13 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>56893</v>
+        <v>56899</v>
       </c>
       <c r="E31" t="n">
         <v>3790</v>
       </c>
       <c r="F31" t="n">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G31" s="2" t="n">
         <v>44656</v>
@@ -1449,10 +1449,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>90422</v>
+        <v>90429</v>
       </c>
       <c r="E32" t="n">
-        <v>5604</v>
+        <v>5605</v>
       </c>
       <c r="F32" t="n">
         <v>237</v>
@@ -1481,10 +1481,10 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>60470</v>
+        <v>60491</v>
       </c>
       <c r="E33" t="n">
-        <v>3001</v>
+        <v>3003</v>
       </c>
       <c r="F33" t="n">
         <v>96</v>
@@ -1513,7 +1513,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>38118</v>
+        <v>38123</v>
       </c>
       <c r="E34" t="n">
         <v>1578</v>
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>48581</v>
+        <v>48583</v>
       </c>
       <c r="E35" t="n">
         <v>1830</v>
@@ -1577,7 +1577,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>34244</v>
+        <v>34251</v>
       </c>
       <c r="E36" t="n">
         <v>1407</v>
@@ -1609,10 +1609,10 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>345049</v>
+        <v>345107</v>
       </c>
       <c r="E37" t="n">
-        <v>17206</v>
+        <v>17208</v>
       </c>
       <c r="F37" t="n">
         <v>579</v>
@@ -1641,7 +1641,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>57962</v>
+        <v>57968</v>
       </c>
       <c r="E38" t="n">
         <v>3205</v>
@@ -1673,10 +1673,10 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>615843</v>
+        <v>615916</v>
       </c>
       <c r="E39" t="n">
-        <v>38837</v>
+        <v>38842</v>
       </c>
       <c r="F39" t="n">
         <v>624</v>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>14453</v>
+        <v>14455</v>
       </c>
       <c r="E40" t="n">
         <v>595</v>
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>202179</v>
+        <v>202189</v>
       </c>
       <c r="E41" t="n">
         <v>9096</v>
@@ -1769,7 +1769,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>49348</v>
+        <v>49350</v>
       </c>
       <c r="E42" t="n">
         <v>2593</v>
@@ -1801,7 +1801,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>22627</v>
+        <v>22628</v>
       </c>
       <c r="E43" t="n">
         <v>939</v>
@@ -1833,7 +1833,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>62636</v>
+        <v>62642</v>
       </c>
       <c r="E44" t="n">
         <v>3095</v>
@@ -1865,7 +1865,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>120146</v>
+        <v>120155</v>
       </c>
       <c r="E45" t="n">
         <v>2987</v>
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>75662</v>
+        <v>75674</v>
       </c>
       <c r="E46" t="n">
         <v>4221</v>
@@ -1929,7 +1929,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>200150</v>
+        <v>200159</v>
       </c>
       <c r="E47" t="n">
         <v>7862</v>
@@ -1961,7 +1961,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>31329</v>
+        <v>31332</v>
       </c>
       <c r="E48" t="n">
         <v>1122</v>
@@ -1993,10 +1993,10 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>106463</v>
+        <v>106487</v>
       </c>
       <c r="E49" t="n">
-        <v>6846</v>
+        <v>6849</v>
       </c>
       <c r="F49" t="n">
         <v>328</v>
@@ -2025,10 +2025,10 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>138134</v>
+        <v>138178</v>
       </c>
       <c r="E50" t="n">
-        <v>7609</v>
+        <v>7612</v>
       </c>
       <c r="F50" t="n">
         <v>204</v>
@@ -2089,7 +2089,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>80338</v>
+        <v>80344</v>
       </c>
       <c r="E52" t="n">
         <v>3475</v>
@@ -2121,10 +2121,10 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>2090444</v>
+        <v>2091641</v>
       </c>
       <c r="E53" t="n">
-        <v>95800</v>
+        <v>95821</v>
       </c>
       <c r="F53" t="n">
         <v>1798</v>
@@ -2153,10 +2153,10 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>272423</v>
+        <v>272456</v>
       </c>
       <c r="E54" t="n">
-        <v>9892</v>
+        <v>9895</v>
       </c>
       <c r="F54" t="n">
         <v>483</v>
@@ -2185,10 +2185,10 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>688398</v>
+        <v>688545</v>
       </c>
       <c r="E55" t="n">
-        <v>19712</v>
+        <v>19715</v>
       </c>
       <c r="F55" t="n">
         <v>950</v>
@@ -2217,7 +2217,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>495227</v>
+        <v>495251</v>
       </c>
       <c r="E56" t="n">
         <v>22037</v>
@@ -2249,10 +2249,10 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>98466</v>
+        <v>98474</v>
       </c>
       <c r="E57" t="n">
-        <v>4635</v>
+        <v>4636</v>
       </c>
       <c r="F57" t="n">
         <v>176</v>
@@ -2281,7 +2281,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>49533</v>
+        <v>49538</v>
       </c>
       <c r="E58" t="n">
         <v>3044</v>
@@ -2313,10 +2313,10 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>315591</v>
+        <v>315626</v>
       </c>
       <c r="E59" t="n">
-        <v>15788</v>
+        <v>15789</v>
       </c>
       <c r="F59" t="n">
         <v>352</v>
@@ -2345,7 +2345,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>52519</v>
+        <v>52533</v>
       </c>
       <c r="E60" t="n">
         <v>1368</v>
@@ -2377,10 +2377,10 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>200153</v>
+        <v>200220</v>
       </c>
       <c r="E61" t="n">
-        <v>10162</v>
+        <v>10166</v>
       </c>
       <c r="F61" t="n">
         <v>253</v>
@@ -2441,10 +2441,10 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>74975</v>
+        <v>74990</v>
       </c>
       <c r="E63" t="n">
-        <v>4011</v>
+        <v>4012</v>
       </c>
       <c r="F63" t="n">
         <v>145</v>
@@ -2473,10 +2473,10 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>188418</v>
+        <v>188439</v>
       </c>
       <c r="E64" t="n">
-        <v>8963</v>
+        <v>8964</v>
       </c>
       <c r="F64" t="n">
         <v>257</v>
@@ -2505,7 +2505,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>29735</v>
+        <v>29738</v>
       </c>
       <c r="E65" t="n">
         <v>1518</v>
@@ -2537,7 +2537,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>30357</v>
+        <v>30361</v>
       </c>
       <c r="E66" t="n">
         <v>870</v>
@@ -2569,7 +2569,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>62872</v>
+        <v>62873</v>
       </c>
       <c r="E67" t="n">
         <v>1851</v>
@@ -2601,10 +2601,10 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>262710</v>
+        <v>262754</v>
       </c>
       <c r="E68" t="n">
-        <v>10574</v>
+        <v>10577</v>
       </c>
       <c r="F68" t="n">
         <v>270</v>
@@ -2665,10 +2665,10 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>50625</v>
+        <v>50631</v>
       </c>
       <c r="E70" t="n">
-        <v>2359</v>
+        <v>2358</v>
       </c>
       <c r="F70" t="n">
         <v>134</v>
@@ -2697,7 +2697,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>22742</v>
+        <v>22743</v>
       </c>
       <c r="E71" t="n">
         <v>653</v>
@@ -2729,7 +2729,7 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>81570</v>
+        <v>81599</v>
       </c>
       <c r="E72" t="n">
         <v>1691</v>
@@ -2761,10 +2761,10 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>3149041</v>
+        <v>3149552</v>
       </c>
       <c r="E73" t="n">
-        <v>177522</v>
+        <v>177544</v>
       </c>
       <c r="F73" t="n">
         <v>2523</v>
@@ -2793,7 +2793,7 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>82864</v>
+        <v>82877</v>
       </c>
       <c r="E74" t="n">
         <v>1865</v>
@@ -2825,10 +2825,10 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>452346</v>
+        <v>452420</v>
       </c>
       <c r="E75" t="n">
-        <v>13948</v>
+        <v>13949</v>
       </c>
       <c r="F75" t="n">
         <v>588</v>
@@ -2857,10 +2857,10 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>2133995</v>
+        <v>2136500</v>
       </c>
       <c r="E76" t="n">
-        <v>75932</v>
+        <v>75989</v>
       </c>
       <c r="F76" t="n">
         <v>1709</v>
@@ -2889,7 +2889,7 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>53710</v>
+        <v>53732</v>
       </c>
       <c r="E77" t="n">
         <v>964</v>
@@ -2921,7 +2921,7 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>330574</v>
+        <v>330607</v>
       </c>
       <c r="E78" t="n">
         <v>11499</v>
@@ -2953,7 +2953,7 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>27384</v>
+        <v>27390</v>
       </c>
       <c r="E79" t="n">
         <v>830</v>
@@ -3049,7 +3049,7 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>6129</v>
+        <v>6130</v>
       </c>
       <c r="E82" t="n">
         <v>220</v>
@@ -3081,7 +3081,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>50537</v>
+        <v>50550</v>
       </c>
       <c r="E83" t="n">
         <v>1481</v>
@@ -3145,7 +3145,7 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>5722</v>
+        <v>5723</v>
       </c>
       <c r="E85" t="n">
         <v>294</v>
@@ -3177,7 +3177,7 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>61115</v>
+        <v>61121</v>
       </c>
       <c r="E86" t="n">
         <v>2251</v>
@@ -3209,7 +3209,7 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>292377</v>
+        <v>292389</v>
       </c>
       <c r="E87" t="n">
         <v>7693</v>
@@ -3241,7 +3241,7 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>99319</v>
+        <v>99327</v>
       </c>
       <c r="E88" t="n">
         <v>4045</v>
@@ -3273,7 +3273,7 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>15607</v>
+        <v>15609</v>
       </c>
       <c r="E89" t="n">
         <v>355</v>
@@ -3305,10 +3305,10 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>467191</v>
+        <v>467223</v>
       </c>
       <c r="E90" t="n">
-        <v>21381</v>
+        <v>21383</v>
       </c>
       <c r="F90" t="n">
         <v>631</v>
@@ -3369,7 +3369,7 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>11375</v>
+        <v>11376</v>
       </c>
       <c r="E92" t="n">
         <v>300</v>
@@ -3401,7 +3401,7 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>14471</v>
+        <v>14472</v>
       </c>
       <c r="E93" t="n">
         <v>300</v>
@@ -3433,7 +3433,7 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>38364</v>
+        <v>38385</v>
       </c>
       <c r="E94" t="n">
         <v>1985</v>
@@ -3465,7 +3465,7 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>18704</v>
+        <v>18705</v>
       </c>
       <c r="E95" t="n">
         <v>368</v>
@@ -3497,7 +3497,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>15701</v>
+        <v>15703</v>
       </c>
       <c r="E96" t="n">
         <v>478</v>
@@ -3529,7 +3529,7 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>104425</v>
+        <v>104440</v>
       </c>
       <c r="E97" t="n">
         <v>2686</v>
@@ -3561,7 +3561,7 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>9535</v>
+        <v>9536</v>
       </c>
       <c r="E98" t="n">
         <v>251</v>
@@ -3593,7 +3593,7 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>230100</v>
+        <v>230116</v>
       </c>
       <c r="E99" t="n">
         <v>6180</v>
@@ -3657,7 +3657,7 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>29064</v>
+        <v>29067</v>
       </c>
       <c r="E101" t="n">
         <v>1934</v>
@@ -3753,7 +3753,7 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>12468</v>
+        <v>12469</v>
       </c>
       <c r="E104" t="n">
         <v>322</v>
@@ -3785,7 +3785,7 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>14677</v>
+        <v>14678</v>
       </c>
       <c r="E105" t="n">
         <v>318</v>
@@ -3849,7 +3849,7 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>14545</v>
+        <v>14546</v>
       </c>
       <c r="E107" t="n">
         <v>341</v>
@@ -3881,7 +3881,7 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>89505</v>
+        <v>89522</v>
       </c>
       <c r="E108" t="n">
         <v>2666</v>
@@ -3945,7 +3945,7 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>30132</v>
+        <v>30136</v>
       </c>
       <c r="E110" t="n">
         <v>890</v>
@@ -3977,7 +3977,7 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>22526</v>
+        <v>22528</v>
       </c>
       <c r="E111" t="n">
         <v>1189</v>
@@ -4009,10 +4009,10 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>227648</v>
+        <v>227673</v>
       </c>
       <c r="E112" t="n">
-        <v>7857</v>
+        <v>7859</v>
       </c>
       <c r="F112" t="n">
         <v>302</v>
@@ -4041,7 +4041,7 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>12891</v>
+        <v>12894</v>
       </c>
       <c r="E113" t="n">
         <v>350</v>
@@ -4073,7 +4073,7 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>19224</v>
+        <v>19233</v>
       </c>
       <c r="E114" t="n">
         <v>1016</v>
@@ -4105,10 +4105,10 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>68428</v>
+        <v>68434</v>
       </c>
       <c r="E115" t="n">
-        <v>3548</v>
+        <v>3549</v>
       </c>
       <c r="F115" t="n">
         <v>204</v>
@@ -4169,10 +4169,10 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>106735</v>
+        <v>106745</v>
       </c>
       <c r="E117" t="n">
-        <v>6326</v>
+        <v>6327</v>
       </c>
       <c r="F117" t="n">
         <v>233</v>
@@ -4201,7 +4201,7 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>6784</v>
+        <v>6785</v>
       </c>
       <c r="E118" t="n">
         <v>190</v>
@@ -4233,7 +4233,7 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>15389</v>
+        <v>15392</v>
       </c>
       <c r="E119" t="n">
         <v>441</v>
@@ -4265,7 +4265,7 @@
         </is>
       </c>
       <c r="D120" t="n">
-        <v>29864</v>
+        <v>29869</v>
       </c>
       <c r="E120" t="n">
         <v>994</v>
@@ -4297,10 +4297,10 @@
         </is>
       </c>
       <c r="D121" t="n">
-        <v>369452</v>
+        <v>369532</v>
       </c>
       <c r="E121" t="n">
-        <v>16886</v>
+        <v>16890</v>
       </c>
       <c r="F121" t="n">
         <v>656</v>
@@ -4329,7 +4329,7 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>21594</v>
+        <v>21595</v>
       </c>
       <c r="E122" t="n">
         <v>351</v>

</xml_diff>